<commit_message>
chg: Updated tasking for MSN 16
</commit_message>
<xml_diff>
--- a/Files/OP URGENT FURY Frequency and Callsign master list.xlsx
+++ b/Files/OP URGENT FURY Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="758">
   <si>
     <t>AWACS</t>
   </si>
@@ -2262,6 +2262,42 @@
   </si>
   <si>
     <t>COMM 2 (VHF)</t>
+  </si>
+  <si>
+    <t>F16</t>
+  </si>
+  <si>
+    <t>WHITE 5</t>
+  </si>
+  <si>
+    <t>AMBER 4</t>
+  </si>
+  <si>
+    <t>ORANGE 3</t>
+  </si>
+  <si>
+    <t>PINK 5</t>
+  </si>
+  <si>
+    <t>BROWN 5</t>
+  </si>
+  <si>
+    <t>VIOLET 8</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>BROWN 7</t>
+  </si>
+  <si>
+    <t>GREY 8</t>
+  </si>
+  <si>
+    <t>YELLOW 11</t>
+  </si>
+  <si>
+    <t>CORAL 3</t>
   </si>
 </sst>
 </file>
@@ -3173,10 +3209,10 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3575,10 +3611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:AF44"/>
+  <dimension ref="B3:AF51"/>
   <sheetViews>
-    <sheetView topLeftCell="I25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3674,21 +3710,21 @@
       <c r="S4" s="34" t="s">
         <v>546</v>
       </c>
-      <c r="V4" s="101" t="s">
+      <c r="V4" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="101"/>
-      <c r="X4" s="101"/>
-      <c r="Z4" s="101" t="s">
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Z4" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="101"/>
-      <c r="AB4" s="101"/>
-      <c r="AD4" s="101" t="s">
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="100"/>
+      <c r="AD4" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="AE4" s="101"/>
-      <c r="AF4" s="101"/>
+      <c r="AE4" s="100"/>
+      <c r="AF4" s="100"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="60" t="s">
@@ -3878,7 +3914,7 @@
       <c r="L7" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="42" t="s">
+      <c r="M7" s="17" t="s">
         <v>70</v>
       </c>
       <c r="N7" s="61" t="s">
@@ -3933,7 +3969,7 @@
       <c r="D8" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="16" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="41" t="s">
@@ -4065,7 +4101,7 @@
       <c r="F10" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="16" t="s">
         <v>100</v>
       </c>
       <c r="H10" s="42" t="s">
@@ -4132,7 +4168,7 @@
       <c r="I11" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="16" t="s">
         <v>115</v>
       </c>
       <c r="K11" s="42" t="s">
@@ -4167,11 +4203,11 @@
       <c r="X11" t="s">
         <v>513</v>
       </c>
-      <c r="Z11" s="101" t="s">
+      <c r="Z11" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="AA11" s="101"/>
-      <c r="AB11" s="101"/>
+      <c r="AA11" s="100"/>
+      <c r="AB11" s="100"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="60" t="s">
@@ -4189,7 +4225,7 @@
       <c r="F12" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="17" t="s">
         <v>124</v>
       </c>
       <c r="H12" s="42" t="s">
@@ -4259,13 +4295,13 @@
       <c r="F13" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="17" t="s">
         <v>136</v>
       </c>
       <c r="H13" s="41" t="s">
         <v>457</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="I13" s="16" t="s">
         <v>137</v>
       </c>
       <c r="J13" s="12" t="s">
@@ -4338,7 +4374,7 @@
       <c r="I14" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="J14" s="41" t="s">
+      <c r="J14" s="17" t="s">
         <v>150</v>
       </c>
       <c r="K14" s="17" t="s">
@@ -4390,7 +4426,7 @@
       <c r="E15" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="16" t="s">
         <v>158</v>
       </c>
       <c r="G15" s="42" t="s">
@@ -4598,11 +4634,11 @@
         <v>312</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="101" t="s">
+      <c r="R18" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="101"/>
-      <c r="T18" s="101"/>
+      <c r="S18" s="100"/>
+      <c r="T18" s="100"/>
     </row>
     <row r="19" spans="2:32">
       <c r="B19" s="60" t="s">
@@ -4665,13 +4701,13 @@
       <c r="X19" s="103"/>
       <c r="Y19" s="103"/>
       <c r="Z19" s="104"/>
-      <c r="AB19" s="101" t="s">
+      <c r="AB19" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="101"/>
-      <c r="AD19" s="101"/>
-      <c r="AE19" s="101"/>
-      <c r="AF19" s="101"/>
+      <c r="AC19" s="100"/>
+      <c r="AD19" s="100"/>
+      <c r="AE19" s="100"/>
+      <c r="AF19" s="100"/>
     </row>
     <row r="20" spans="2:32">
       <c r="B20" s="60" t="s">
@@ -4683,7 +4719,7 @@
       <c r="D20" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="17" t="s">
         <v>205</v>
       </c>
       <c r="F20" s="42" t="s">
@@ -5054,11 +5090,11 @@
       </c>
       <c r="O25" s="55"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="101" t="s">
+      <c r="R25" s="100" t="s">
         <v>563</v>
       </c>
-      <c r="S25" s="101"/>
-      <c r="T25" s="101"/>
+      <c r="S25" s="100"/>
+      <c r="T25" s="100"/>
     </row>
     <row r="26" spans="2:32">
       <c r="B26" s="60" t="s">
@@ -5209,33 +5245,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="100" t="s">
         <v>313</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
-      <c r="J31" s="101" t="s">
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="100"/>
+      <c r="J31" s="100" t="s">
         <v>314</v>
       </c>
-      <c r="K31" s="101"/>
-      <c r="L31" s="101"/>
-      <c r="M31" s="101"/>
-      <c r="N31" s="101"/>
-      <c r="O31" s="101"/>
-      <c r="P31" s="101"/>
-      <c r="U31" s="101" t="s">
+      <c r="K31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="U31" s="100" t="s">
         <v>296</v>
       </c>
-      <c r="V31" s="101"/>
-      <c r="W31" s="101"/>
-      <c r="X31" s="101"/>
-      <c r="Y31" s="101"/>
-      <c r="Z31" s="101"/>
-      <c r="AA31" s="101"/>
+      <c r="V31" s="100"/>
+      <c r="W31" s="100"/>
+      <c r="X31" s="100"/>
+      <c r="Y31" s="100"/>
+      <c r="Z31" s="100"/>
+      <c r="AA31" s="100"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="54" t="s">
@@ -5684,15 +5720,15 @@
       <c r="F39" t="s">
         <v>653</v>
       </c>
-      <c r="J39" s="100" t="s">
+      <c r="J39" s="101" t="s">
         <v>494</v>
       </c>
-      <c r="K39" s="100"/>
-      <c r="L39" s="100"/>
-      <c r="M39" s="100"/>
-      <c r="N39" s="100"/>
-      <c r="O39" s="100"/>
-      <c r="P39" s="100"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="101"/>
+      <c r="M39" s="101"/>
+      <c r="N39" s="101"/>
+      <c r="O39" s="101"/>
+      <c r="P39" s="101"/>
       <c r="T39">
         <v>7</v>
       </c>
@@ -5828,8 +5864,98 @@
         <v>727</v>
       </c>
     </row>
+    <row r="45" spans="2:27">
+      <c r="W45" t="s">
+        <v>753</v>
+      </c>
+      <c r="X45" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>754</v>
+      </c>
+      <c r="Z45" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="46" spans="2:27">
+      <c r="W46" t="s">
+        <v>753</v>
+      </c>
+      <c r="X46" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>755</v>
+      </c>
+      <c r="Z46" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="49" spans="23:27">
+      <c r="W49" t="s">
+        <v>746</v>
+      </c>
+      <c r="X49" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>747</v>
+      </c>
+      <c r="Z49" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="50" spans="23:27">
+      <c r="W50" t="s">
+        <v>746</v>
+      </c>
+      <c r="X50" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>748</v>
+      </c>
+      <c r="Z50" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="51" spans="23:27">
+      <c r="W51" t="s">
+        <v>746</v>
+      </c>
+      <c r="X51" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>749</v>
+      </c>
+      <c r="Z51" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>752</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="U31:AA31"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="V19:Z19"/>
+    <mergeCell ref="J31:P31"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="AB19:AF19"/>
@@ -5837,11 +5963,6 @@
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="R25:T25"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="U31:AA31"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="V19:Z19"/>
-    <mergeCell ref="J31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5852,7 +5973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chg: Added F14 presets / updated NOTAM with aircraft start locations
</commit_message>
<xml_diff>
--- a/Files/OP URGENT FURY Frequency and Callsign master list.xlsx
+++ b/Files/OP URGENT FURY Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -13,18 +13,19 @@
     <sheet name="A10 presets" sheetId="5" r:id="rId4"/>
     <sheet name="Ka-50 presets" sheetId="6" r:id="rId5"/>
     <sheet name="MI-8 presets" sheetId="7" r:id="rId6"/>
-    <sheet name="FA-18 Hornet Presets" sheetId="10" r:id="rId7"/>
-    <sheet name="AV-8B Presets" sheetId="8" r:id="rId8"/>
-    <sheet name="AJS-37 Presets" sheetId="9" r:id="rId9"/>
-    <sheet name="AI Callsigns" sheetId="11" r:id="rId10"/>
-    <sheet name="F-16 Presets" sheetId="12" r:id="rId11"/>
+    <sheet name="F-14 Presets" sheetId="13" r:id="rId7"/>
+    <sheet name="FA-18 Hornet Presets" sheetId="10" r:id="rId8"/>
+    <sheet name="AV-8B Presets" sheetId="8" r:id="rId9"/>
+    <sheet name="AJS-37 Presets" sheetId="9" r:id="rId10"/>
+    <sheet name="AI Callsigns" sheetId="11" r:id="rId11"/>
+    <sheet name="F-16 Presets" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="761">
   <si>
     <t>AWACS</t>
   </si>
@@ -2298,6 +2299,15 @@
   </si>
   <si>
     <t>CORAL 3</t>
+  </si>
+  <si>
+    <t>F-14 presets OPUF V1.0</t>
+  </si>
+  <si>
+    <t>119.25</t>
+  </si>
+  <si>
+    <t>YELLOW 8</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +3014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3209,10 +3219,10 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3317,6 +3327,16 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3613,8 +3633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA46" sqref="AA46"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3710,21 +3730,21 @@
       <c r="S4" s="34" t="s">
         <v>546</v>
       </c>
-      <c r="V4" s="100" t="s">
+      <c r="V4" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="100"/>
-      <c r="X4" s="100"/>
-      <c r="Z4" s="100" t="s">
+      <c r="W4" s="101"/>
+      <c r="X4" s="101"/>
+      <c r="Z4" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="100"/>
-      <c r="AB4" s="100"/>
-      <c r="AD4" s="100" t="s">
+      <c r="AA4" s="101"/>
+      <c r="AB4" s="101"/>
+      <c r="AD4" s="101" t="s">
         <v>294</v>
       </c>
-      <c r="AE4" s="100"/>
-      <c r="AF4" s="100"/>
+      <c r="AE4" s="101"/>
+      <c r="AF4" s="101"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="60" t="s">
@@ -4203,11 +4223,11 @@
       <c r="X11" t="s">
         <v>513</v>
       </c>
-      <c r="Z11" s="100" t="s">
+      <c r="Z11" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="AA11" s="100"/>
-      <c r="AB11" s="100"/>
+      <c r="AA11" s="101"/>
+      <c r="AB11" s="101"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="60" t="s">
@@ -4634,11 +4654,11 @@
         <v>312</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="100" t="s">
+      <c r="R18" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="100"/>
-      <c r="T18" s="100"/>
+      <c r="S18" s="101"/>
+      <c r="T18" s="101"/>
     </row>
     <row r="19" spans="2:32">
       <c r="B19" s="60" t="s">
@@ -4701,13 +4721,13 @@
       <c r="X19" s="103"/>
       <c r="Y19" s="103"/>
       <c r="Z19" s="104"/>
-      <c r="AB19" s="100" t="s">
+      <c r="AB19" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="100"/>
-      <c r="AD19" s="100"/>
-      <c r="AE19" s="100"/>
-      <c r="AF19" s="100"/>
+      <c r="AC19" s="101"/>
+      <c r="AD19" s="101"/>
+      <c r="AE19" s="101"/>
+      <c r="AF19" s="101"/>
     </row>
     <row r="20" spans="2:32">
       <c r="B20" s="60" t="s">
@@ -5090,11 +5110,11 @@
       </c>
       <c r="O25" s="55"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="100" t="s">
+      <c r="R25" s="101" t="s">
         <v>563</v>
       </c>
-      <c r="S25" s="100"/>
-      <c r="T25" s="100"/>
+      <c r="S25" s="101"/>
+      <c r="T25" s="101"/>
     </row>
     <row r="26" spans="2:32">
       <c r="B26" s="60" t="s">
@@ -5245,33 +5265,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="101" t="s">
         <v>313</v>
       </c>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="100"/>
-      <c r="J31" s="100" t="s">
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="J31" s="101" t="s">
         <v>314</v>
       </c>
-      <c r="K31" s="100"/>
-      <c r="L31" s="100"/>
-      <c r="M31" s="100"/>
-      <c r="N31" s="100"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="100"/>
-      <c r="U31" s="100" t="s">
+      <c r="K31" s="101"/>
+      <c r="L31" s="101"/>
+      <c r="M31" s="101"/>
+      <c r="N31" s="101"/>
+      <c r="O31" s="101"/>
+      <c r="P31" s="101"/>
+      <c r="U31" s="101" t="s">
         <v>296</v>
       </c>
-      <c r="V31" s="100"/>
-      <c r="W31" s="100"/>
-      <c r="X31" s="100"/>
-      <c r="Y31" s="100"/>
-      <c r="Z31" s="100"/>
-      <c r="AA31" s="100"/>
+      <c r="V31" s="101"/>
+      <c r="W31" s="101"/>
+      <c r="X31" s="101"/>
+      <c r="Y31" s="101"/>
+      <c r="Z31" s="101"/>
+      <c r="AA31" s="101"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="54" t="s">
@@ -5720,15 +5740,15 @@
       <c r="F39" t="s">
         <v>653</v>
       </c>
-      <c r="J39" s="101" t="s">
+      <c r="J39" s="100" t="s">
         <v>494</v>
       </c>
-      <c r="K39" s="101"/>
-      <c r="L39" s="101"/>
-      <c r="M39" s="101"/>
-      <c r="N39" s="101"/>
-      <c r="O39" s="101"/>
-      <c r="P39" s="101"/>
+      <c r="K39" s="100"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="100"/>
+      <c r="N39" s="100"/>
+      <c r="O39" s="100"/>
+      <c r="P39" s="100"/>
       <c r="T39">
         <v>7</v>
       </c>
@@ -5894,7 +5914,7 @@
       <c r="Z46" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="AA46" t="s">
+      <c r="AA46" s="2" t="s">
         <v>757</v>
       </c>
     </row>
@@ -5951,11 +5971,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="U31:AA31"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="V19:Z19"/>
-    <mergeCell ref="J31:P31"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="AB19:AF19"/>
@@ -5963,6 +5978,11 @@
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="R25:T25"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="U31:AA31"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="V19:Z19"/>
+    <mergeCell ref="J31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5970,6 +5990,255 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="125" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="B2" s="126" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="B4" s="47" t="s">
+        <v>379</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="B5" s="47" t="s">
+        <v>381</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
+      <c r="B6" s="47" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
+      <c r="B7" s="47" t="s">
+        <v>385</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="B8" s="47" t="s">
+        <v>388</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>389</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
+      <c r="B9" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="B10" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="46"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="B14" s="126" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="B15" s="46"/>
+      <c r="C15" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75">
+      <c r="B16" s="47" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="46"/>
+    </row>
+    <row r="17" spans="2:5" ht="18.75">
+      <c r="B17" s="47" t="s">
+        <v>381</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>382</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="E17" s="46"/>
+    </row>
+    <row r="18" spans="2:5" ht="18.75">
+      <c r="B18" s="47" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>384</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="46"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75">
+      <c r="B19" s="47" t="s">
+        <v>385</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>386</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>396</v>
+      </c>
+      <c r="E19" s="46"/>
+    </row>
+    <row r="20" spans="2:5" ht="18.75">
+      <c r="B20" s="47" t="s">
+        <v>388</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>389</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>397</v>
+      </c>
+      <c r="E20" s="46"/>
+    </row>
+    <row r="21" spans="2:5" ht="18.75">
+      <c r="B21" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>398</v>
+      </c>
+      <c r="E21" s="46"/>
+    </row>
+    <row r="22" spans="2:5" ht="18.75">
+      <c r="B22" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="E22" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B14:E14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O39"/>
   <sheetViews>
@@ -6968,7 +7237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H52"/>
   <sheetViews>
@@ -10187,10 +10456,742 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="105" t="s">
+        <v>758</v>
+      </c>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A2" s="136"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="137"/>
+    </row>
+    <row r="3" spans="1:8" ht="23.25">
+      <c r="A3" s="119" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="119" t="s">
+        <v>400</v>
+      </c>
+      <c r="F3" s="120"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="122"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A4" s="84">
+        <v>1</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>715</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E4" s="84">
+        <v>1</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>546</v>
+      </c>
+      <c r="G4" s="85"/>
+      <c r="H4" s="86" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A5" s="84">
+        <v>2</v>
+      </c>
+      <c r="B5" s="83" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="85" t="s">
+        <v>716</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E5" s="84">
+        <v>2</v>
+      </c>
+      <c r="F5" s="83" t="s">
+        <v>547</v>
+      </c>
+      <c r="G5" s="85"/>
+      <c r="H5" s="86" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A6" s="84">
+        <v>3</v>
+      </c>
+      <c r="B6" s="83" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>717</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E6" s="84">
+        <v>3</v>
+      </c>
+      <c r="F6" s="83" t="s">
+        <v>526</v>
+      </c>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A7" s="84">
+        <v>4</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="85" t="s">
+        <v>718</v>
+      </c>
+      <c r="D7" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E7" s="84">
+        <v>4</v>
+      </c>
+      <c r="F7" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="85" t="s">
+        <v>498</v>
+      </c>
+      <c r="H7" s="87" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A8" s="84">
+        <v>5</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="85" t="s">
+        <v>472</v>
+      </c>
+      <c r="D8" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E8" s="84">
+        <v>5</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="85" t="s">
+        <v>721</v>
+      </c>
+      <c r="H8" s="86" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A9" s="84">
+        <v>6</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="85" t="s">
+        <v>540</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E9" s="84">
+        <v>6</v>
+      </c>
+      <c r="F9" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="85" t="s">
+        <v>502</v>
+      </c>
+      <c r="H9" s="86" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A10" s="84">
+        <v>7</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="85" t="s">
+        <v>541</v>
+      </c>
+      <c r="D10" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E10" s="84">
+        <v>7</v>
+      </c>
+      <c r="F10" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="85" t="s">
+        <v>499</v>
+      </c>
+      <c r="H10" s="86" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A11" s="84">
+        <v>8</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="85" t="s">
+        <v>542</v>
+      </c>
+      <c r="D11" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E11" s="84">
+        <v>8</v>
+      </c>
+      <c r="F11" s="83" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="85" t="s">
+        <v>501</v>
+      </c>
+      <c r="H11" s="86" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A12" s="84">
+        <v>9</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="85" t="s">
+        <v>543</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E12" s="84">
+        <v>9</v>
+      </c>
+      <c r="F12" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="85" t="s">
+        <v>393</v>
+      </c>
+      <c r="H12" s="86" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A13" s="84">
+        <v>10</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="85" t="s">
+        <v>544</v>
+      </c>
+      <c r="D13" s="86" t="s">
+        <v>401</v>
+      </c>
+      <c r="E13" s="84">
+        <v>10</v>
+      </c>
+      <c r="F13" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="85" t="s">
+        <v>503</v>
+      </c>
+      <c r="H13" s="86" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A14" s="84">
+        <v>11</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="85" t="s">
+        <v>538</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>506</v>
+      </c>
+      <c r="E14" s="84">
+        <v>11</v>
+      </c>
+      <c r="F14" s="83" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="85" t="s">
+        <v>513</v>
+      </c>
+      <c r="H14" s="86" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A15" s="84">
+        <v>12</v>
+      </c>
+      <c r="B15" s="83" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="85" t="s">
+        <v>719</v>
+      </c>
+      <c r="D15" s="86" t="s">
+        <v>507</v>
+      </c>
+      <c r="E15" s="84">
+        <v>12</v>
+      </c>
+      <c r="F15" s="83" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="85" t="s">
+        <v>519</v>
+      </c>
+      <c r="H15" s="86" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A16" s="84">
+        <v>13</v>
+      </c>
+      <c r="B16" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="85" t="s">
+        <v>760</v>
+      </c>
+      <c r="D16" s="87" t="s">
+        <v>345</v>
+      </c>
+      <c r="E16" s="84">
+        <v>13</v>
+      </c>
+      <c r="F16" s="83" t="s">
+        <v>201</v>
+      </c>
+      <c r="G16" s="85" t="s">
+        <v>520</v>
+      </c>
+      <c r="H16" s="86" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A17" s="84">
+        <v>14</v>
+      </c>
+      <c r="B17" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>760</v>
+      </c>
+      <c r="D17" s="87" t="s">
+        <v>345</v>
+      </c>
+      <c r="E17" s="84">
+        <v>14</v>
+      </c>
+      <c r="F17" s="83" t="s">
+        <v>235</v>
+      </c>
+      <c r="G17" s="85" t="s">
+        <v>522</v>
+      </c>
+      <c r="H17" s="86" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A18" s="84">
+        <v>15</v>
+      </c>
+      <c r="B18" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="85" t="s">
+        <v>556</v>
+      </c>
+      <c r="D18" s="86" t="s">
+        <v>559</v>
+      </c>
+      <c r="E18" s="84">
+        <v>15</v>
+      </c>
+      <c r="F18" s="83" t="s">
+        <v>552</v>
+      </c>
+      <c r="G18" s="85"/>
+      <c r="H18" s="86" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A19" s="84">
+        <v>16</v>
+      </c>
+      <c r="B19" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="85" t="s">
+        <v>557</v>
+      </c>
+      <c r="D19" s="86" t="s">
+        <v>560</v>
+      </c>
+      <c r="E19" s="84">
+        <v>16</v>
+      </c>
+      <c r="F19" s="83" t="s">
+        <v>553</v>
+      </c>
+      <c r="G19" s="85"/>
+      <c r="H19" s="86" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A20" s="84">
+        <v>17</v>
+      </c>
+      <c r="B20" s="83" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="85" t="s">
+        <v>720</v>
+      </c>
+      <c r="D20" s="86" t="s">
+        <v>561</v>
+      </c>
+      <c r="E20" s="84">
+        <v>17</v>
+      </c>
+      <c r="F20" s="83" t="s">
+        <v>565</v>
+      </c>
+      <c r="G20" s="85"/>
+      <c r="H20" s="87" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A21" s="84">
+        <v>18</v>
+      </c>
+      <c r="B21" s="83" t="s">
+        <v>568</v>
+      </c>
+      <c r="C21" s="85"/>
+      <c r="D21" s="86" t="s">
+        <v>567</v>
+      </c>
+      <c r="E21" s="84">
+        <v>18</v>
+      </c>
+      <c r="F21" s="83" t="s">
+        <v>566</v>
+      </c>
+      <c r="G21" s="85"/>
+      <c r="H21" s="87" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A22" s="84">
+        <v>19</v>
+      </c>
+      <c r="B22" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="85" t="s">
+        <v>504</v>
+      </c>
+      <c r="D22" s="87" t="s">
+        <v>356</v>
+      </c>
+      <c r="E22" s="84">
+        <v>19</v>
+      </c>
+      <c r="F22" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="85" t="s">
+        <v>504</v>
+      </c>
+      <c r="H22" s="86" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A23" s="84">
+        <v>20</v>
+      </c>
+      <c r="B23" s="83" t="s">
+        <v>569</v>
+      </c>
+      <c r="C23" s="85"/>
+      <c r="D23" s="86" t="s">
+        <v>567</v>
+      </c>
+      <c r="E23" s="84">
+        <v>20</v>
+      </c>
+      <c r="F23" s="83" t="s">
+        <v>528</v>
+      </c>
+      <c r="G23" s="85"/>
+      <c r="H23" s="86" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A24" s="138"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="84">
+        <v>21</v>
+      </c>
+      <c r="F24" s="83" t="s">
+        <v>759</v>
+      </c>
+      <c r="G24" s="85" t="s">
+        <v>529</v>
+      </c>
+      <c r="H24" s="87" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A25" s="138"/>
+      <c r="B25" s="139"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="139"/>
+      <c r="E25" s="84">
+        <v>22</v>
+      </c>
+      <c r="F25" s="83" t="s">
+        <v>270</v>
+      </c>
+      <c r="G25" s="85" t="s">
+        <v>534</v>
+      </c>
+      <c r="H25" s="87" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A26" s="138"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="84">
+        <v>23</v>
+      </c>
+      <c r="F26" s="83">
+        <v>260</v>
+      </c>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A27" s="138"/>
+      <c r="B27" s="139"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="139"/>
+      <c r="E27" s="84">
+        <v>24</v>
+      </c>
+      <c r="F27" s="83">
+        <v>270</v>
+      </c>
+      <c r="G27" s="85"/>
+      <c r="H27" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A28" s="138"/>
+      <c r="B28" s="139"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="84">
+        <v>25</v>
+      </c>
+      <c r="F28" s="83">
+        <v>255</v>
+      </c>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A29" s="138"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="84">
+        <v>26</v>
+      </c>
+      <c r="F29" s="83">
+        <v>259</v>
+      </c>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A30" s="138"/>
+      <c r="B30" s="139"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="84">
+        <v>27</v>
+      </c>
+      <c r="F30" s="83">
+        <v>262</v>
+      </c>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A31" s="138"/>
+      <c r="B31" s="139"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="84">
+        <v>28</v>
+      </c>
+      <c r="F31" s="83">
+        <v>257</v>
+      </c>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A32" s="138"/>
+      <c r="B32" s="139"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="139"/>
+      <c r="E32" s="84">
+        <v>29</v>
+      </c>
+      <c r="F32" s="83">
+        <v>253</v>
+      </c>
+      <c r="G32" s="85"/>
+      <c r="H32" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A33" s="140"/>
+      <c r="B33" s="141"/>
+      <c r="C33" s="141"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="84">
+        <v>30</v>
+      </c>
+      <c r="F33" s="83">
+        <v>263</v>
+      </c>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H23"/>
+      <selection activeCell="C16" sqref="C16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10753,7 +11754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F29"/>
   <sheetViews>
@@ -11323,253 +12324,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="125" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="126" t="s">
-        <v>378</v>
-      </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47" t="s">
-        <v>322</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>330</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75">
-      <c r="B4" s="47" t="s">
-        <v>379</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>380</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75">
-      <c r="B5" s="47" t="s">
-        <v>381</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>382</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>320</v>
-      </c>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75">
-      <c r="B6" s="47" t="s">
-        <v>383</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>384</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="46"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75">
-      <c r="B7" s="47" t="s">
-        <v>385</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>386</v>
-      </c>
-      <c r="D7" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75">
-      <c r="B8" s="47" t="s">
-        <v>388</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>389</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75">
-      <c r="B9" s="47" t="s">
-        <v>391</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>392</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.75">
-      <c r="B10" s="47" t="s">
-        <v>394</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>299</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="E10" s="46"/>
-    </row>
-    <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="126" t="s">
-        <v>395</v>
-      </c>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75">
-      <c r="B15" s="46"/>
-      <c r="C15" s="47" t="s">
-        <v>322</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>330</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75">
-      <c r="B16" s="47" t="s">
-        <v>379</v>
-      </c>
-      <c r="C16" s="46" t="s">
-        <v>380</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="46"/>
-    </row>
-    <row r="17" spans="2:5" ht="18.75">
-      <c r="B17" s="47" t="s">
-        <v>381</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>382</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>320</v>
-      </c>
-      <c r="E17" s="46"/>
-    </row>
-    <row r="18" spans="2:5" ht="18.75">
-      <c r="B18" s="47" t="s">
-        <v>383</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>384</v>
-      </c>
-      <c r="D18" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="46"/>
-    </row>
-    <row r="19" spans="2:5" ht="18.75">
-      <c r="B19" s="47" t="s">
-        <v>385</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>386</v>
-      </c>
-      <c r="D19" s="49" t="s">
-        <v>396</v>
-      </c>
-      <c r="E19" s="46"/>
-    </row>
-    <row r="20" spans="2:5" ht="18.75">
-      <c r="B20" s="47" t="s">
-        <v>388</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>389</v>
-      </c>
-      <c r="D20" s="49" t="s">
-        <v>397</v>
-      </c>
-      <c r="E20" s="46"/>
-    </row>
-    <row r="21" spans="2:5" ht="18.75">
-      <c r="B21" s="47" t="s">
-        <v>391</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>392</v>
-      </c>
-      <c r="D21" s="49" t="s">
-        <v>398</v>
-      </c>
-      <c r="E21" s="46"/>
-    </row>
-    <row r="22" spans="2:5" ht="18.75">
-      <c r="B22" s="47" t="s">
-        <v>394</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>299</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="E22" s="46"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B14:E14"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>